<commit_message>
Actualizar casos y estatus
</commit_message>
<xml_diff>
--- a/Casos Cartera/Administración.xlsx
+++ b/Casos Cartera/Administración.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" tabRatio="787" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" tabRatio="787" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Alta crédito manual" sheetId="15" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="228">
   <si>
     <t>Nombre CP</t>
   </si>
@@ -55,67 +55,6 @@
     <t>Modificar</t>
   </si>
   <si>
-    <t>TC_Cartera_ProcesosSeleccion_CartaGuia</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesosSeleccion_ExportarExcel</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesosSeleccion_CartaGuiaPolitica</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesosSeleccion_IncluirPagares</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesosSeleccion_ExcluirPagares</t>
-  </si>
-  <si>
-    <t>Validar inclusión de pagares que cumple con las políticas aplicadas en los criterios de selección</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Selección de creditos (afianza), seleccionar opcion si del filtro excluidos, hacer clic en boton incorporar, hacer clic en boton si</t>
-  </si>
-  <si>
-    <t>Inclusion de pagare de manera exitosa</t>
-  </si>
-  <si>
-    <t>Validar emision de carta guia con pagares que cumple con las políticas aplicadas en los criterios de selección</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Selección de creditos (afianza), hacer clic en boton crear carta guia</t>
-  </si>
-  <si>
-    <t>Emisión de carta guia con pagares que cumple con las políticas aplicadas en los criterios de selección</t>
-  </si>
-  <si>
-    <t>Validar descarga de archivo excel con pagares que cumple y no cumplen con las políticas aplicadas en los criterios de selección</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Selección de creditos (afianza), seleccionar opcion con politica del filtro Política Selección, hacer clic en boton exportar a excel, luego, seleccionar opcion sin politica del filtro Política Selección, hacer clic en boton exportar a excel</t>
-  </si>
-  <si>
-    <t>Descarga de archivo excel, visualizando registro según criterios seleccionados</t>
-  </si>
-  <si>
-    <t>Validar emision de carta guia con pagares que no cumple con las políticas aplicadas en los criterios de selección</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Selección de creditos (afianza), seleccionar opcion sin politica del filtro Política Selección, hacer clic en boton crear carta guia</t>
-  </si>
-  <si>
-    <t>Emisión de carta guia con pagares que no cumple con las políticas aplicadas en los criterios 
-de selección, la selección de pagares queda a criterio del usuario para emitir carta</t>
-  </si>
-  <si>
-    <t>Validar exclusión de pagares que cumplen y no cumplen con las políticas aplicadas en los criterios de selección</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Selección de creditos (afianza), seleccionar opcion sin politica del filtro Política Selección, hacer clic en boton desmarcar credito, hacer clic en boton si, luego, seleccionar opcion sin politica del filtro Política Selección, hacer clic en boton desmarcar credito, hacer clic en boton si</t>
-  </si>
-  <si>
-    <t>Exclusion de pagare de manera exitosa</t>
-  </si>
-  <si>
     <t>TC_Cartera_ProcesoXML_OfertaTD</t>
   </si>
   <si>
@@ -173,78 +112,6 @@
     <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Centralización Créditos Nuevos, hacer clic en botón generar contabilización</t>
   </si>
   <si>
-    <t>Se genera archivo excel con los créditos que posean cobertura</t>
-  </si>
-  <si>
-    <t>Se genera archivo excel con los créditos que no posean cobertura</t>
-  </si>
-  <si>
-    <t>Se genera archivo excel con todos los créditos</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesosLSD_ConCobertura</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesosLSD_SinCobertura</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesosLSD_Todas</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesosLSD_SeguroSinCobertura</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesosLSD_AdministradorGarantias</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesosLSD_CorredoraSeguros</t>
-  </si>
-  <si>
-    <t>Validar emisión de planilla excel, la cual contiene los créditos con seguro de desgravamen, seleccionando los que tengan cobertura</t>
-  </si>
-  <si>
-    <t>Validar emisión de planilla excel, la cual contiene los créditos con seguro de desgravamen, seleccionando los que no tengan cobertura</t>
-  </si>
-  <si>
-    <t>Validar emisión de planilla excel, la cual contiene los créditos con seguro de desgravamen, seleccionando todos los registros.</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub Liquidación Seguro Desgravamen, seleccionar opción con cobertura del combo cobertura, hacer clic en boton exportar a excel</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub Liquidación Seguro Desgravamen, seleccionar opción sin cobertura del combo cobertura, hacer clic en boton exportar a excel</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub Liquidación Seguro Desgravamen, seleccionar opción Todos del combo cobertura, hacer clic en boton exportar a excel</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub Liquidación Seguro Desgravamen, hacer clic en boton Seguro sin Cobertura</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub Liquidación Seguro Desgravamen, hacer clic en boton Administrador Garantías</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub Liquidación Seguro Desgravamen, hacer clic en botón Corredora de Seguros</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validar envío de archivo a directorio FTP, de liquidación de seguro sin cobertura </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validar envío de archivo por correo con la información de liquidación de seguro con cobertura </t>
-  </si>
-  <si>
-    <t>Validar envío de archivo por correo con la información de liquidación de seguro con cobertura y nombre de corredora</t>
-  </si>
-  <si>
-    <t>Envío de archivo a directorio FTP de manera exitosa</t>
-  </si>
-  <si>
-    <t>Envío de archivo a correo de liquidación de seguro con cobertura de manera exitosa</t>
-  </si>
-  <si>
-    <t>Envío de archivo a correo de liquidación de seguro con cobertura y nombre de corredora de manera exitosa</t>
-  </si>
-  <si>
     <t>TC_Cartera_SBIFD92_DescargarArchivo</t>
   </si>
   <si>
@@ -647,9 +514,6 @@
     <t>Tipo dato</t>
   </si>
   <si>
-    <t xml:space="preserve">Numerico </t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -681,6 +545,177 @@
   </si>
   <si>
     <t>No Aplica</t>
+  </si>
+  <si>
+    <t>Exportar a Excel</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_ANumericoIgual</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_ANumericoMayor</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_ANumericoMenor</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_AFechaMayorIgual</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_AFechaMenorIgual</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_ACaracterDistino</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_ACaracterNoAplica</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_ENumericoIgual</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_ENumericoMayor</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_ENumericoMenor</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_EFechaMayorIgual</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_EFechaMenorIgual</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_ECaracterDistino</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_ECaracterNoAplica</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_MNumericoIgual</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_MNumericoMayor</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_MNumericoMenor</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_MFechaMayorIgual</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_MFechaMenorIgual</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_MCaracterDistino</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_MCaracterNoAplica</t>
+  </si>
+  <si>
+    <t>Numerico</t>
+  </si>
+  <si>
+    <t>Registro ingresado de manera exitosa</t>
+  </si>
+  <si>
+    <t>Registro eliminado de manera exitosa</t>
+  </si>
+  <si>
+    <t>Registro modificado de manera exitosa</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionCSC_CriterioExistente</t>
+  </si>
+  <si>
+    <t>Validar ingreso de critero que ya se encuentra en cartera</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito, hacer clic boton agregar, ingresar parámetro ANTIGUEDADLABORALPJ, seleccionar tipo dato numerico, seleccionar operador desde mayor igual 12, operador hasta no aplica, hacer clic en boton confirmar</t>
+  </si>
+  <si>
+    <t>Sistema debe emitir mensaje indicando "Ya existe el registro"</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionExclusionTV_Eliminar</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionExclusionTV_Modificar</t>
+  </si>
+  <si>
+    <t>Tipo Nombre</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionExclusionTV_AgregarVehiculoModificar</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionExclusionTV_AgregarVehiculoEliminar</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionExclusionTV_AgregarVehiculo</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionExclusionTV_ConsolidadoError</t>
+  </si>
+  <si>
+    <t>Validar funcionalidad agregar exlcusión tipo vehículo, considerando enlace tipo nombre para modificar registro.</t>
+  </si>
+  <si>
+    <t>Validar funcionalidad agregar exlcusión tipo vehículo, considerando enlace Tipo nombre para eliminar registro.</t>
+  </si>
+  <si>
+    <t>Validar funcionalidad agregar exlcusión tipo vehículo, seleccionando tipo ID 2 para ingresar el nuevo registro.</t>
+  </si>
+  <si>
+    <t>Validar funcionalidad eliminar exlcusión tipo vehículo, seleccionando registro asociado a tipo nombre camión</t>
+  </si>
+  <si>
+    <t>Validar funcionalidad modificar exlcusión tipo vehículo, seleccionando registro asociado a tipo ID 10.</t>
+  </si>
+  <si>
+    <t>Validar funcionalidad agregar exclusión tipo vehículo, ingresando datos de registro existente, luego de ello, no se especifica tipo ID</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Exclusión tipo vehículo (Afianza), hacer clic en boton agregar, ingresar tipo ID, hacer clic en campo tipo nombre, hacer clic en boton confirmar, seleccionar registro y hacer clic en enlace tipo nombre, hacer clic en boton modificar, editar datos del registro, hacer clic en boton confirmar.</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Exclusión tipo vehículo (Afianza), hacer clic en boton agregar, ingresar tipo ID, hacer clic en campo tipo nombre, hacer clic en boton confirmar.</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Exclusión tipo vehículo (Afianza), hacer clic en boton agregar, ingresar tipo IDl, hacer clic en campo tipo nombre seleccionar rango de morosidad, hacer clic en boton confirmar, seleccionar registro y hacer clic en enlace tipo nombre, hacer clic en boton eliminar, hacer clic en boton confirmar.</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Exclusión tipo vehículo (Afianza), seleccionar registro asociado a tipo nombre camión, hacer clic en boton eliminar, hacer clic en boton confirmar.</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Exclusión tipo vehículo, seleccionar registro asociado a tipo ID 10, hacer clic en boton modificar, editar datos del registro, hacer clic en boton confirmar.</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Exclusión tipo vehículo (Afianza), hacer clic en boton agregar, ingresar tipo ID que se encuentre ya ingresado como excluido, hacer clic en boton confirmar, luego, borrar tipo ID ingresado y hacer clic en boton confirmar.</t>
+  </si>
+  <si>
+    <t>Sistema debe emitir mensaje de error en cada situación planteada</t>
+  </si>
+  <si>
+    <t>Registro de exclusión tipo vehículo de manera exitosa</t>
+  </si>
+  <si>
+    <t>Eliminación de exclusión tipo vehículo de manera exitosa</t>
+  </si>
+  <si>
+    <t>Modificación de exclusión tipo vehículo de manera exitosa</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionTMC_Consulta</t>
+  </si>
+  <si>
+    <t>Validar ingreso al sub modulo tasa máxima convencianal para consultar registros existentes</t>
+  </si>
+  <si>
+    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - Tasa Máxima Convencional, visualizar registros de tasas</t>
+  </si>
+  <si>
+    <t>Consulta de tasas de manera exitosa</t>
   </si>
 </sst>
 </file>
@@ -785,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -868,6 +903,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -898,18 +943,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1231,107 +1275,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>104</v>
+        <v>60</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>99</v>
+        <v>55</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>106</v>
+        <v>62</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1544,65 +1588,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1826,7 +1870,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,65 +1882,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>90</v>
+        <v>46</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>91</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2141,37 +2185,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="41"/>
-      <c r="I1" s="32" t="s">
+      <c r="A1" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="43"/>
+      <c r="G1" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="45"/>
+      <c r="I1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="32" t="s">
+      <c r="K1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
@@ -2182,10 +2226,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>116</v>
+        <v>72</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>6</v>
@@ -2193,10 +2237,10 @@
       <c r="H2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
@@ -2216,7 +2260,7 @@
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="6" t="s">
-        <v>118</v>
+        <v>74</v>
       </c>
       <c r="J3" s="8" t="str">
         <f>CONCATENATE("Validar funcionalidad ",IF(B3=1,$B$2,IF(C3=1,$C$2,IF(D3=1,$D$2))),", considerando el enlace ",IF(E3=1,$E$2,IF(F3=1,$F$2,""))," para realizar la acción de ",IF(G3=1,$G$2,IF(H3=1,$H$2,"")))</f>
@@ -2227,7 +2271,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton agregar, considerar enlace Corriente Nro para realizar la acción de modificar registro</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2248,7 +2292,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>119</v>
+        <v>75</v>
       </c>
       <c r="J4" s="8" t="str">
         <f t="shared" ref="J4:J16" si="0">CONCATENATE("Validar funcionalidad ",IF(B4=1,$B$2,IF(C4=1,$C$2,IF(D4=1,$D$2))),", considerando el enlace ",IF(E4=1,$E$2,IF(F4=1,$F$2,""))," para realizar la acción de ",IF(G4=1,$G$2,IF(H4=1,$H$2,"")))</f>
@@ -2259,7 +2303,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton agregar, considerar enlace Corriente Nro para realizar la acción de eliminar registro</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2280,7 +2324,7 @@
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="6" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="J5" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2291,7 +2335,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton agregar, considerar enlace Banco para realizar la acción de modificar registro</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2312,7 +2356,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="J6" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2323,7 +2367,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton agregar, considerar enlace Banco para realizar la acción de eliminar registro</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2340,17 +2384,17 @@
       <c r="G7" s="4"/>
       <c r="H7" s="7"/>
       <c r="I7" s="6" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="K7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton agregar</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2371,7 +2415,7 @@
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="6" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
       <c r="J8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2382,7 +2426,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton eliminar, considerar enlace Corriente Nro para realizar la acción de modificar registro</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2402,7 +2446,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="J9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2413,7 +2457,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton eliminar, considerar enlace Corriente Nro para realizar la acción de eliminar registro</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2433,7 +2477,7 @@
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="6" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="J10" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2444,7 +2488,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton eliminar, considerar enlace Banco para realizar la acción de modificar registro</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2464,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="J11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2475,7 +2519,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton eliminar, considerar enlace Banco para realizar la acción de eliminar registro</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2491,17 +2535,17 @@
       <c r="G12" s="4"/>
       <c r="H12" s="7"/>
       <c r="I12" s="6" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="K12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton eliminar</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2520,7 +2564,7 @@
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="6" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="J13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2531,7 +2575,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton modificar, considerar enlace Corriente Nro para realizar la acción de modificar registro</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2550,7 +2594,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="J14" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2561,7 +2605,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton modificar, considerar enlace Corriente Nro para realizar la acción de eliminar registro</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2580,7 +2624,7 @@
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="6" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="J15" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2591,7 +2635,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton modificar, considerar enlace Banco para realizar la acción de modificar registro</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2610,7 +2654,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="J16" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2621,7 +2665,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton modificar, considerar enlace Banco para realizar la acción de eliminar registro</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2636,17 +2680,17 @@
       <c r="G17" s="4"/>
       <c r="H17" s="7"/>
       <c r="I17" s="6" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="K17" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton modificar</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2828,16 +2872,16 @@
       <c r="G32" s="4"/>
       <c r="H32" s="7"/>
       <c r="I32" s="6" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -3081,39 +3125,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
+      <c r="A1" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="25" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="I1" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="45"/>
+      <c r="H1" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="32" t="s">
+      <c r="K1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="9" customFormat="1" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
@@ -3124,7 +3168,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -3132,11 +3176,11 @@
       <c r="G2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
@@ -3156,16 +3200,16 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="6" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>153</v>
+        <v>109</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>156</v>
+        <v>112</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3186,16 +3230,16 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="6" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>157</v>
+        <v>113</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>164</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3214,16 +3258,16 @@
         <v>1</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>158</v>
+        <v>114</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>165</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3240,16 +3284,16 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="6" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>159</v>
+        <v>115</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>166</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3268,16 +3312,16 @@
         <v>1</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>149</v>
+        <v>105</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>160</v>
+        <v>116</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3293,16 +3337,16 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="6" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>168</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3320,16 +3364,16 @@
         <v>1</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>173</v>
+        <v>129</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>169</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3373,16 +3417,16 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="6" t="s">
-        <v>174</v>
+        <v>130</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>175</v>
+        <v>131</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>176</v>
+        <v>132</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3820,51 +3864,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4090,8 +4134,8 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="9" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L7" sqref="L7"/>
+      <pane xSplit="9" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4111,39 +4155,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="39"/>
+      <c r="A1" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="43"/>
       <c r="E1" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="40" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="41"/>
-      <c r="H1" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="I1" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="45"/>
+      <c r="H1" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="32" t="s">
+      <c r="K1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
@@ -4154,7 +4198,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -4162,11 +4206,11 @@
       <c r="G2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
@@ -4186,16 +4230,16 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="6" t="s">
-        <v>180</v>
+        <v>136</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>192</v>
+        <v>148</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4216,16 +4260,16 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="6" t="s">
-        <v>182</v>
+        <v>138</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>193</v>
+        <v>149</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4244,20 +4288,22 @@
         <v>1</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>183</v>
+        <v>139</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>188</v>
+        <v>144</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>199</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4">
         <v>1</v>
@@ -4270,20 +4316,22 @@
         <v>1</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>195</v>
+        <v>151</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>201</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="7">
@@ -4296,16 +4344,16 @@
         <v>1</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>196</v>
+        <v>152</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -4331,16 +4379,16 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="6" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>191</v>
+        <v>147</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>198</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4830,108 +4878,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G10" sqref="G9:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.42578125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="126.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="255.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="101" style="6" customWidth="1"/>
+    <col min="2" max="2" width="94" style="8" customWidth="1"/>
+    <col min="3" max="3" width="151.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>10</v>
+        <v>224</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>12</v>
+        <v>225</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>226</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>14</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="A4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>23</v>
-      </c>
+      <c r="A5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>26</v>
-      </c>
+      <c r="A7" s="6"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
@@ -5155,65 +5171,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="9" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5434,11 +5450,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y52"/>
+  <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="22" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="23" topLeftCell="X1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5454,132 +5470,136 @@
     <col min="11" max="12" width="3.85546875" customWidth="1"/>
     <col min="13" max="13" width="3.5703125" customWidth="1"/>
     <col min="14" max="14" width="4.140625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="2.7109375" style="42" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" style="42" customWidth="1"/>
-    <col min="17" max="17" width="3.5703125" style="42" customWidth="1"/>
-    <col min="18" max="18" width="2.85546875" style="42" customWidth="1"/>
-    <col min="19" max="19" width="3.42578125" style="42" customWidth="1"/>
-    <col min="20" max="20" width="3.5703125" style="42" customWidth="1"/>
-    <col min="21" max="21" width="3.85546875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="58.5703125" style="2" customWidth="1"/>
-    <col min="23" max="23" width="160.85546875" style="8" customWidth="1"/>
-    <col min="24" max="24" width="255.42578125" style="6" customWidth="1"/>
-    <col min="25" max="25" width="85.5703125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="2.7109375" style="34" customWidth="1"/>
+    <col min="16" max="16" width="3.7109375" style="34" customWidth="1"/>
+    <col min="17" max="17" width="3.5703125" style="34" customWidth="1"/>
+    <col min="18" max="18" width="2.85546875" style="34" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" style="34" customWidth="1"/>
+    <col min="20" max="20" width="3.5703125" style="34" customWidth="1"/>
+    <col min="21" max="22" width="3.85546875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="58.5703125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="163.42578125" style="8" customWidth="1"/>
+    <col min="25" max="25" width="255.42578125" style="6" customWidth="1"/>
+    <col min="26" max="26" width="85.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>113</v>
-      </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40" t="s">
-        <v>207</v>
-      </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="40" t="s">
-        <v>208</v>
-      </c>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="45" t="s">
+    <row r="1" spans="1:26" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="47"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="W1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="W1" s="32" t="s">
+      <c r="X1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" s="32" t="s">
+      <c r="Y1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39"/>
       <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>205</v>
+        <v>160</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>206</v>
+        <v>161</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>209</v>
+        <v>164</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>210</v>
+        <v>165</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>211</v>
+        <v>166</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>212</v>
+        <v>167</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>215</v>
+        <v>170</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>209</v>
+        <v>164</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>210</v>
+        <v>165</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>211</v>
+        <v>166</v>
       </c>
       <c r="R2" s="11" t="s">
-        <v>212</v>
+        <v>167</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
       <c r="U2" s="29" t="s">
-        <v>215</v>
-      </c>
-      <c r="V2" s="35"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-    </row>
-    <row r="3" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="V2" s="37"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="37"/>
+      <c r="Y2" s="37"/>
+      <c r="Z2" s="37"/>
+    </row>
+    <row r="3" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -5611,14 +5631,25 @@
       <c r="U3" s="7">
         <v>1</v>
       </c>
-      <c r="V3" s="46" t="s">
-        <v>118</v>
-      </c>
-      <c r="W3" s="8"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V3" s="7">
+        <v>1</v>
+      </c>
+      <c r="W3" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="X3" s="8" t="str">
+        <f>CONCATENATE("Validad funcionalidad ",IF(B3=1,$B$2,IF(C3=1,$C$2,IF(D3=1,$D$2))),IF(B3=1,", ingresando registro ",IF(C3=1,", seleccionando registro ",IF(D3=1,", seleccionando registro "))),$E$1," ",IF(E3=1,$E$2,IF(F3=1,$F$2,IF(G3=1,$G$2))),"y ",$H$1," ",IF(H3=1,$H$2,IF(I3=1,$I$2,IF(J3=1,$J$2,IF(K3=1,$K$2,IF(L3=1,$L$2,IF(M3=1,$M$2,IF(N3=1,$N$2)))))))," - ",$O$1," ",IF(O3=1,$O$2,IF(P3=1,$P$2,IF(Q3=1,$Q$2,IF(R3=1,$R$2,IF(S3=1,$S$2,IF(T3=1,$T$2,IF(U3=1,$U$2))))))),IF(V3=1,". Considerando la opcion de exportar a excel",""))</f>
+        <v>Validad funcionalidad Agregar, ingresando registro Tipo dato Numericoy Operador Desde Igual - Operador Hasta No Aplica. Considerando la opcion de exportar a excel</v>
+      </c>
+      <c r="Y3" s="6" t="str">
+        <f>CONCATENATE("Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza)",IF(B3=1,", hacer clic en boton agregar e ingresar ",IF(C3=1,", seleccionar registro ",IF(D3=1,", seleccionar registro"))),$E$1," ",IF(E3=1,$E$2,IF(F3=1,$F$2,IF(G3=1,$G$2)))," y ",$H$1," ",IF(H3=1,$H$2,IF(I3=1,$I$2,IF(J3=1,$J$2,IF(K3=1,$K$2,IF(L3=1,$L$2,IF(M3=1,$M$2,IF(N3=1,$N$2)))))))," - ",$O$1," ",IF(O3=1,$O$2,IF(P3=1,$P$2,IF(Q3=1,$Q$2,IF(R3=1,$R$2,IF(S3=1,$S$2,IF(T3=1,$T$2,IF(U3=1,$U$2))))))),IF(C3=1," para eliminar",IF(D3=1," para modificar","")),IF(V3=1,", finalizando con exportar a excel",""))</f>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Numerico y Operador Desde Igual - Operador Hasta No Aplica, finalizando con exportar a excel</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -5650,14 +5681,23 @@
         <v>1</v>
       </c>
       <c r="U4" s="7"/>
-      <c r="V4" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="W4" s="8"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V4" s="7"/>
+      <c r="W4" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="X4" s="8" t="str">
+        <f t="shared" ref="X4:X22" si="0">CONCATENATE("Validad funcionalidad ",IF(B4=1,$B$2,IF(C4=1,$C$2,IF(D4=1,$D$2))),IF(B4=1,", ingresando registro ",IF(C4=1,", seleccionando registro ",IF(D4=1,", seleccionando registro "))),$E$1," ",IF(E4=1,$E$2,IF(F4=1,$F$2,IF(G4=1,$G$2))),"y ",$H$1," ",IF(H4=1,$H$2,IF(I4=1,$I$2,IF(J4=1,$J$2,IF(K4=1,$K$2,IF(L4=1,$L$2,IF(M4=1,$M$2,IF(N4=1,$N$2)))))))," - ",$O$1," ",IF(O4=1,$O$2,IF(P4=1,$P$2,IF(Q4=1,$Q$2,IF(R4=1,$R$2,IF(S4=1,$S$2,IF(T4=1,$T$2,IF(U4=1,$U$2))))))),IF(V4=1,". Considerando la opcion de exportar a excel",""))</f>
+        <v>Validad funcionalidad Agregar, ingresando registro Tipo dato Numericoy Operador Desde Mayor - Operador Hasta Distinto</v>
+      </c>
+      <c r="Y4" s="6" t="str">
+        <f t="shared" ref="Y4:Y23" si="1">CONCATENATE("Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza)",IF(B4=1,", hacer clic en boton agregar e ingresar ",IF(C4=1,", seleccionar registro ",IF(D4=1,", seleccionar registro"))),$E$1," ",IF(E4=1,$E$2,IF(F4=1,$F$2,IF(G4=1,$G$2)))," y ",$H$1," ",IF(H4=1,$H$2,IF(I4=1,$I$2,IF(J4=1,$J$2,IF(K4=1,$K$2,IF(L4=1,$L$2,IF(M4=1,$M$2,IF(N4=1,$N$2)))))))," - ",$O$1," ",IF(O4=1,$O$2,IF(P4=1,$P$2,IF(Q4=1,$Q$2,IF(R4=1,$R$2,IF(S4=1,$S$2,IF(T4=1,$T$2,IF(U4=1,$U$2))))))),IF(C4=1," para eliminar",IF(D4=1," para modificar","")),IF(V4=1,", finalizando con exportar a excel",""))</f>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Numerico y Operador Desde Mayor - Operador Hasta Distinto</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -5689,14 +5729,23 @@
       </c>
       <c r="T5" s="4"/>
       <c r="U5" s="7"/>
-      <c r="V5" s="46" t="s">
-        <v>120</v>
-      </c>
-      <c r="W5" s="8"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-    </row>
-    <row r="6" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V5" s="7"/>
+      <c r="W5" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="X5" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>Validad funcionalidad Agregar, ingresando registro Tipo dato Numericoy Operador Desde Menor - Operador Hasta Menor igual</v>
+      </c>
+      <c r="Y5" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Numerico y Operador Desde Menor - Operador Hasta Menor igual</v>
+      </c>
+      <c r="Z5" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -5705,10 +5754,10 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -5728,14 +5777,25 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="7"/>
-      <c r="V6" s="46" t="s">
-        <v>121</v>
-      </c>
-      <c r="W6" s="8"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V6" s="7">
+        <v>1</v>
+      </c>
+      <c r="W6" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="X6" s="8" t="str">
+        <f>CONCATENATE("Validad funcionalidad ",IF(B6=1,$B$2,IF(C6=1,$C$2,IF(D6=1,$D$2))),IF(B6=1,", ingresando registro ",IF(C6=1,", seleccionando registro ",IF(D6=1,", seleccionando registro "))),$E$1," ",IF(E6=1,$E$2,IF(F6=1,$F$2,IF(G6=1,$G$2)))," y ",$H$1," ",IF(H6=1,$H$2,IF(I6=1,$I$2,IF(J6=1,$J$2,IF(K6=1,$K$2,IF(L6=1,$L$2,IF(M6=1,$M$2,IF(N6=1,$N$2)))))))," - ",$O$1," ",IF(O6=1,$O$2,IF(P6=1,$P$2,IF(Q6=1,$Q$2,IF(R6=1,$R$2,IF(S6=1,$S$2,IF(T6=1,$T$2,IF(U6=1,$U$2))))))),IF(V6=1,". Considerando la opcion de exportar a excel",""))</f>
+        <v>Validad funcionalidad Agregar, ingresando registro Tipo dato Fecha y Operador Desde Mayor igual - Operador Hasta Mayor igual. Considerando la opcion de exportar a excel</v>
+      </c>
+      <c r="Y6" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Fecha y Operador Desde Mayor igual - Operador Hasta Mayor igual, finalizando con exportar a excel</v>
+      </c>
+      <c r="Z6" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>1</v>
       </c>
@@ -5744,10 +5804,10 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -5767,14 +5827,23 @@
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="7"/>
-      <c r="V7" s="46" t="s">
-        <v>122</v>
-      </c>
-      <c r="W7" s="8"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-    </row>
-    <row r="8" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V7" s="7"/>
+      <c r="W7" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="X7" s="8" t="str">
+        <f t="shared" ref="X7:X22" si="2">CONCATENATE("Validad funcionalidad ",IF(B7=1,$B$2,IF(C7=1,$C$2,IF(D7=1,$D$2))),IF(B7=1,", ingresando registro ",IF(C7=1,", seleccionando registro ",IF(D7=1,", seleccionando registro "))),$E$1," ",IF(E7=1,$E$2,IF(F7=1,$F$2,IF(G7=1,$G$2)))," y ",$H$1," ",IF(H7=1,$H$2,IF(I7=1,$I$2,IF(J7=1,$J$2,IF(K7=1,$K$2,IF(L7=1,$L$2,IF(M7=1,$M$2,IF(N7=1,$N$2)))))))," - ",$O$1," ",IF(O7=1,$O$2,IF(P7=1,$P$2,IF(Q7=1,$Q$2,IF(R7=1,$R$2,IF(S7=1,$S$2,IF(T7=1,$T$2,IF(U7=1,$U$2))))))),IF(V7=1,". Considerando la opcion de exportar a excel",""))</f>
+        <v>Validad funcionalidad Agregar, ingresando registro Tipo dato Fecha y Operador Desde Menor igual - Operador Hasta Menor</v>
+      </c>
+      <c r="Y7" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Fecha y Operador Desde Menor igual - Operador Hasta Menor</v>
+      </c>
+      <c r="Z7" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>1</v>
       </c>
@@ -5783,11 +5852,11 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="7"/>
+      <c r="G8" s="7">
+        <v>1</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -5806,14 +5875,23 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="7"/>
-      <c r="V8" s="46" t="s">
-        <v>125</v>
-      </c>
-      <c r="W8" s="8"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="15"/>
-    </row>
-    <row r="9" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V8" s="7"/>
+      <c r="W8" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="X8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Agregar, ingresando registro Tipo dato Carácter y Operador Desde Distinto - Operador Hasta Mayor</v>
+      </c>
+      <c r="Y8" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Carácter y Operador Desde Distinto - Operador Hasta Mayor</v>
+      </c>
+      <c r="Z8" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>1</v>
       </c>
@@ -5822,11 +5900,11 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="7"/>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -5845,21 +5923,32 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="7"/>
-      <c r="V9" s="46" t="s">
-        <v>126</v>
-      </c>
-      <c r="W9" s="8"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="15"/>
-    </row>
-    <row r="10" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V9" s="7">
+        <v>1</v>
+      </c>
+      <c r="W9" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="X9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Agregar, ingresando registro Tipo dato Carácter y Operador Desde No Aplica - Operador Hasta Igual. Considerando la opcion de exportar a excel</v>
+      </c>
+      <c r="Y9" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Carácter y Operador Desde No Aplica - Operador Hasta Igual, finalizando con exportar a excel</v>
+      </c>
+      <c r="Z9" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>1</v>
       </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
       <c r="D10" s="7"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4">
@@ -5884,21 +5973,30 @@
       <c r="U10" s="7">
         <v>1</v>
       </c>
-      <c r="V10" s="46" t="s">
-        <v>127</v>
-      </c>
-      <c r="W10" s="8"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="15"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V10" s="7"/>
+      <c r="W10" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="X10" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Eliminar, seleccionando registro Tipo dato Fecha y Operador Desde Igual - Operador Hasta No Aplica</v>
+      </c>
+      <c r="Y10" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Fecha y Operador Desde Igual - Operador Hasta No Aplica para eliminar</v>
+      </c>
+      <c r="Z10" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>1</v>
       </c>
-      <c r="B11" s="4">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
       <c r="D11" s="7"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4">
@@ -5923,19 +6021,30 @@
         <v>1</v>
       </c>
       <c r="U11" s="7"/>
-      <c r="V11" s="46" t="s">
-        <v>128</v>
-      </c>
-      <c r="Y11" s="15"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V11" s="7"/>
+      <c r="W11" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="X11" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Eliminar, seleccionando registro Tipo dato Fecha y Operador Desde Mayor - Operador Hasta Distinto</v>
+      </c>
+      <c r="Y11" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Fecha y Operador Desde Mayor - Operador Hasta Distinto para eliminar</v>
+      </c>
+      <c r="Z11" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>1</v>
       </c>
-      <c r="B12" s="4">
-        <v>1</v>
-      </c>
-      <c r="C12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
       <c r="D12" s="7"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4">
@@ -5960,24 +6069,38 @@
       </c>
       <c r="T12" s="4"/>
       <c r="U12" s="7"/>
-      <c r="V12" s="46" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y12" s="15"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V12" s="7">
+        <v>1</v>
+      </c>
+      <c r="W12" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="X12" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Eliminar, seleccionando registro Tipo dato Fecha y Operador Desde Menor - Operador Hasta Menor igual. Considerando la opcion de exportar a excel</v>
+      </c>
+      <c r="Y12" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Fecha y Operador Desde Menor - Operador Hasta Menor igual para eliminar, finalizando con exportar a excel</v>
+      </c>
+      <c r="Z12" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>1</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4">
         <v>1</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="4">
-        <v>1</v>
-      </c>
-      <c r="G13" s="7"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="7">
+        <v>1</v>
+      </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
@@ -5996,24 +6119,36 @@
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="7"/>
-      <c r="V13" s="46" t="s">
-        <v>129</v>
-      </c>
-      <c r="Y13" s="15"/>
-    </row>
-    <row r="14" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V13" s="7"/>
+      <c r="W13" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="X13" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Eliminar, seleccionando registro Tipo dato Carácter y Operador Desde Mayor igual - Operador Hasta Mayor igual</v>
+      </c>
+      <c r="Y13" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Carácter y Operador Desde Mayor igual - Operador Hasta Mayor igual para eliminar</v>
+      </c>
+      <c r="Z13" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>1</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4">
         <v>1</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="4">
-        <v>1</v>
-      </c>
-      <c r="G14" s="7"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="7">
+        <v>1</v>
+      </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
@@ -6032,25 +6167,35 @@
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="7"/>
-      <c r="V14" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="W14" s="8"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="15"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V14" s="7"/>
+      <c r="W14" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="X14" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Eliminar, seleccionando registro Tipo dato Carácter y Operador Desde Menor igual - Operador Hasta Menor</v>
+      </c>
+      <c r="Y14" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Carácter y Operador Desde Menor igual - Operador Hasta Menor para eliminar</v>
+      </c>
+      <c r="Z14" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>1</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4">
         <v>1</v>
       </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4">
-        <v>1</v>
-      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4"/>
       <c r="G15" s="7"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -6070,23 +6215,37 @@
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
       <c r="U15" s="7"/>
-      <c r="V15" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y15" s="15"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V15" s="7">
+        <v>1</v>
+      </c>
+      <c r="W15" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="X15" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Eliminar, seleccionando registro Tipo dato Numerico y Operador Desde Distinto - Operador Hasta Mayor. Considerando la opcion de exportar a excel</v>
+      </c>
+      <c r="Y15" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Numerico y Operador Desde Distinto - Operador Hasta Mayor para eliminar, finalizando con exportar a excel</v>
+      </c>
+      <c r="Z15" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>1</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4">
-        <v>1</v>
-      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4"/>
       <c r="G16" s="7"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -6106,19 +6265,30 @@
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
       <c r="U16" s="7"/>
-      <c r="V16" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="Y16" s="15"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V16" s="7"/>
+      <c r="W16" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="X16" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Eliminar, seleccionando registro Tipo dato Numerico y Operador Desde No Aplica - Operador Hasta Igual</v>
+      </c>
+      <c r="Y16" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Numerico y Operador Desde No Aplica - Operador Hasta Igual para eliminar</v>
+      </c>
+      <c r="Z16" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>1</v>
       </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="D17" s="7"/>
+      <c r="B17" s="4"/>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="7">
@@ -6142,16 +6312,28 @@
       <c r="U17" s="7">
         <v>1</v>
       </c>
-      <c r="V17" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y17" s="15"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V17" s="7"/>
+      <c r="W17" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="X17" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Modificar, seleccionando registro Tipo dato Carácter y Operador Desde Igual - Operador Hasta No Aplica</v>
+      </c>
+      <c r="Y17" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Carácter y Operador Desde Igual - Operador Hasta No Aplica para modificar</v>
+      </c>
+      <c r="Z17" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>1</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="4"/>
+      <c r="D18" s="7">
         <v>1</v>
       </c>
       <c r="E18" s="4"/>
@@ -6177,16 +6359,32 @@
         <v>1</v>
       </c>
       <c r="U18" s="7"/>
-      <c r="V18" s="46"/>
-    </row>
-    <row r="19" spans="1:25" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V18" s="7">
+        <v>1</v>
+      </c>
+      <c r="W18" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="X18" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Modificar, seleccionando registro Tipo dato Carácter y Operador Desde Mayor - Operador Hasta Distinto. Considerando la opcion de exportar a excel</v>
+      </c>
+      <c r="Y18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Carácter y Operador Desde Mayor - Operador Hasta Distinto para modificar, finalizando con exportar a excel</v>
+      </c>
+      <c r="Z18" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>1</v>
       </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="21"/>
+      <c r="B19" s="4"/>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="7">
@@ -6210,24 +6408,35 @@
       </c>
       <c r="T19" s="4"/>
       <c r="U19" s="7"/>
-      <c r="V19" s="46"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="15"/>
-    </row>
-    <row r="20" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V19" s="7"/>
+      <c r="W19" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="X19" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Modificar, seleccionando registro Tipo dato Carácter y Operador Desde Menor - Operador Hasta Menor igual</v>
+      </c>
+      <c r="Y19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Carácter y Operador Desde Menor - Operador Hasta Menor igual para modificar</v>
+      </c>
+      <c r="Z19" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>1</v>
       </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="D20" s="7"/>
+      <c r="B20" s="4"/>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="7">
-        <v>1</v>
-      </c>
+      <c r="F20" s="4">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
@@ -6246,25 +6455,36 @@
       <c r="S20" s="4"/>
       <c r="T20" s="4"/>
       <c r="U20" s="7"/>
-      <c r="V20" s="46"/>
-      <c r="W20" s="8"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="15"/>
-    </row>
-    <row r="21" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="7"/>
+      <c r="W20" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="X20" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Modificar, seleccionando registro Tipo dato Fecha y Operador Desde Mayor igual - Operador Hasta Mayor igual</v>
+      </c>
+      <c r="Y20" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Fecha y Operador Desde Mayor igual - Operador Hasta Mayor igual para modificar</v>
+      </c>
+      <c r="Z20" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>1</v>
       </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
+      <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="7"/>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="7">
-        <v>1</v>
-      </c>
+      <c r="F21" s="4">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
@@ -6283,25 +6503,38 @@
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
       <c r="U21" s="7"/>
-      <c r="V21" s="46"/>
-      <c r="W21" s="8"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="15"/>
-    </row>
-    <row r="22" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V21" s="7">
+        <v>1</v>
+      </c>
+      <c r="W21" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="X21" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Modificar, seleccionando registro Tipo dato Fecha y Operador Desde Menor igual - Operador Hasta Menor. Considerando la opcion de exportar a excel</v>
+      </c>
+      <c r="Y21" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Fecha y Operador Desde Menor igual - Operador Hasta Menor para modificar, finalizando con exportar a excel</v>
+      </c>
+      <c r="Z21" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>1</v>
       </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
+      <c r="B22" s="4"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="4"/>
+      <c r="D22" s="7">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="7">
-        <v>1</v>
-      </c>
+      <c r="G22" s="7"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
@@ -6320,25 +6553,36 @@
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
       <c r="U22" s="7"/>
-      <c r="V22" s="46"/>
-      <c r="W22" s="8"/>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-    </row>
-    <row r="23" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V22" s="7"/>
+      <c r="W22" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="X22" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Validad funcionalidad Modificar, seleccionando registro Tipo dato Numerico y Operador Desde Distinto - Operador Hasta Mayor</v>
+      </c>
+      <c r="Y22" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Numerico y Operador Desde Distinto - Operador Hasta Mayor para modificar</v>
+      </c>
+      <c r="Z22" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>1</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
+      <c r="B23" s="4"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="4"/>
+      <c r="D23" s="7">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="7">
-        <v>1</v>
-      </c>
+      <c r="G23" s="7"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -6357,12 +6601,23 @@
       <c r="S23" s="4"/>
       <c r="T23" s="4"/>
       <c r="U23" s="7"/>
-      <c r="V23" s="46"/>
-      <c r="W23" s="8"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-    </row>
-    <row r="24" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V23" s="7"/>
+      <c r="W23" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="X23" s="8" t="str">
+        <f>CONCATENATE("Validad funcionalidad ",IF(B23=1,$B$2,IF(C23=1,$C$2,IF(D23=1,$D$2))),IF(B23=1,", ingresando registro ",IF(C23=1,", seleccionando registro ",IF(D23=1,", seleccionando registro "))),$E$1," ",IF(E23=1,$E$2,IF(F23=1,$F$2,IF(G23=1,$G$2)))," y ",$H$1," ",IF(H23=1,$H$2,IF(I23=1,$I$2,IF(J23=1,$J$2,IF(K23=1,$K$2,IF(L23=1,$L$2,IF(M23=1,$M$2,IF(N23=1,$N$2)))))))," - ",$O$1," ",IF(O23=1,$O$2,IF(P23=1,$P$2,IF(Q23=1,$Q$2,IF(R23=1,$R$2,IF(S23=1,$S$2,IF(T23=1,$T$2,IF(U23=1,$U$2))))))),IF(V23=1,". Considerando la opcion de exportar a excel",""))</f>
+        <v>Validad funcionalidad Modificar, seleccionando registro Tipo dato Numerico y Operador Desde No Aplica - Operador Hasta Igual</v>
+      </c>
+      <c r="Y23" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Numerico y Operador Desde No Aplica - Operador Hasta Igual para modificar</v>
+      </c>
+      <c r="Z23" s="15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -6384,12 +6639,13 @@
       <c r="S24" s="4"/>
       <c r="T24" s="4"/>
       <c r="U24" s="7"/>
-      <c r="V24" s="46"/>
-      <c r="W24" s="8"/>
-      <c r="X24" s="6"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="35"/>
+      <c r="X24" s="8"/>
       <c r="Y24" s="6"/>
-    </row>
-    <row r="25" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z24" s="6"/>
+    </row>
+    <row r="25" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -6411,12 +6667,13 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
       <c r="U25" s="7"/>
-      <c r="V25" s="46"/>
-      <c r="W25" s="8"/>
-      <c r="X25" s="6"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="35"/>
+      <c r="X25" s="8"/>
       <c r="Y25" s="6"/>
-    </row>
-    <row r="26" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z25" s="6"/>
+    </row>
+    <row r="26" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -6438,12 +6695,13 @@
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
       <c r="U26" s="7"/>
-      <c r="V26" s="46"/>
-      <c r="W26" s="8"/>
-      <c r="X26" s="6"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="35"/>
+      <c r="X26" s="8"/>
       <c r="Y26" s="6"/>
-    </row>
-    <row r="27" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z26" s="6"/>
+    </row>
+    <row r="27" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -6465,12 +6723,13 @@
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
       <c r="U27" s="7"/>
-      <c r="V27" s="46"/>
-      <c r="W27" s="8"/>
-      <c r="X27" s="18"/>
-      <c r="Y27" s="6"/>
-    </row>
-    <row r="28" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V27" s="7"/>
+      <c r="W27" s="35"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="18"/>
+      <c r="Z27" s="6"/>
+    </row>
+    <row r="28" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -6492,13 +6751,15 @@
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
       <c r="U28" s="7"/>
-      <c r="V28" s="46"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="6"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="35"/>
+      <c r="X28" s="8"/>
       <c r="Y28" s="6"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z28" s="6"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
+      <c r="C29" s="4"/>
       <c r="D29" s="7"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
@@ -6517,10 +6778,12 @@
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
       <c r="U29" s="7"/>
-      <c r="V29" s="46"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V29" s="7"/>
+      <c r="W29" s="35"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
+      <c r="C30" s="4"/>
       <c r="D30" s="7"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
@@ -6539,10 +6802,12 @@
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
       <c r="U30" s="7"/>
-      <c r="V30" s="46"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V30" s="7"/>
+      <c r="W30" s="35"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
+      <c r="C31" s="4"/>
       <c r="D31" s="7"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -6561,10 +6826,12 @@
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
       <c r="U31" s="7"/>
-      <c r="V31" s="46"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V31" s="7"/>
+      <c r="W31" s="35"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="7"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -6583,21 +6850,23 @@
       <c r="S32" s="4"/>
       <c r="T32" s="4"/>
       <c r="U32" s="7"/>
-      <c r="V32" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="W32" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="X32" s="6" t="s">
-        <v>139</v>
+      <c r="V32" s="7"/>
+      <c r="W32" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="X32" s="8" t="s">
+        <v>198</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="Z32" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
+      <c r="C33" s="4"/>
       <c r="D33" s="7"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -6616,10 +6885,12 @@
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
       <c r="U33" s="7"/>
-      <c r="V33" s="46"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V33" s="7"/>
+      <c r="W33" s="35"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
+      <c r="C34" s="4"/>
       <c r="D34" s="7"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -6638,10 +6909,12 @@
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>
       <c r="U34" s="7"/>
-      <c r="V34" s="46"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V34" s="7"/>
+      <c r="W34" s="35"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
+      <c r="C35" s="4"/>
       <c r="D35" s="7"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -6660,10 +6933,12 @@
       <c r="S35" s="4"/>
       <c r="T35" s="4"/>
       <c r="U35" s="7"/>
-      <c r="V35" s="46"/>
-    </row>
-    <row r="36" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V35" s="7"/>
+      <c r="W35" s="35"/>
+    </row>
+    <row r="36" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
+      <c r="C36" s="4"/>
       <c r="D36" s="7"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -6682,13 +6957,15 @@
       <c r="S36" s="4"/>
       <c r="T36" s="4"/>
       <c r="U36" s="7"/>
-      <c r="V36" s="46"/>
-      <c r="W36" s="8"/>
-      <c r="X36" s="6"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="35"/>
+      <c r="X36" s="8"/>
       <c r="Y36" s="6"/>
-    </row>
-    <row r="37" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z36" s="6"/>
+    </row>
+    <row r="37" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
+      <c r="C37" s="4"/>
       <c r="D37" s="7"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
@@ -6707,13 +6984,15 @@
       <c r="S37" s="4"/>
       <c r="T37" s="4"/>
       <c r="U37" s="7"/>
-      <c r="V37" s="46"/>
-      <c r="W37" s="8"/>
-      <c r="X37" s="6"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="35"/>
+      <c r="X37" s="8"/>
       <c r="Y37" s="6"/>
-    </row>
-    <row r="38" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z37" s="6"/>
+    </row>
+    <row r="38" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
+      <c r="C38" s="4"/>
       <c r="D38" s="7"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -6732,13 +7011,15 @@
       <c r="S38" s="4"/>
       <c r="T38" s="4"/>
       <c r="U38" s="7"/>
-      <c r="V38" s="46"/>
-      <c r="W38" s="8"/>
-      <c r="X38" s="6"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="35"/>
+      <c r="X38" s="8"/>
       <c r="Y38" s="6"/>
-    </row>
-    <row r="39" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z38" s="6"/>
+    </row>
+    <row r="39" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
+      <c r="C39" s="4"/>
       <c r="D39" s="7"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
@@ -6757,16 +7038,18 @@
       <c r="S39" s="4"/>
       <c r="T39" s="4"/>
       <c r="U39" s="7"/>
-      <c r="V39" s="46"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="6"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="35"/>
+      <c r="X39" s="8"/>
       <c r="Y39" s="6"/>
-    </row>
-    <row r="40" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z39" s="6"/>
+    </row>
+    <row r="40" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
+      <c r="C40" s="4"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
       <c r="G40" s="7"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
@@ -6782,13 +7065,15 @@
       <c r="S40" s="4"/>
       <c r="T40" s="4"/>
       <c r="U40" s="7"/>
-      <c r="V40" s="46"/>
-      <c r="W40" s="8"/>
-      <c r="X40" s="6"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="35"/>
+      <c r="X40" s="8"/>
       <c r="Y40" s="6"/>
-    </row>
-    <row r="41" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z40" s="6"/>
+    </row>
+    <row r="41" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
+      <c r="C41" s="4"/>
       <c r="D41" s="7"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -6807,13 +7092,15 @@
       <c r="S41" s="4"/>
       <c r="T41" s="4"/>
       <c r="U41" s="7"/>
-      <c r="V41" s="46"/>
-      <c r="W41" s="8"/>
-      <c r="X41" s="6"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="35"/>
+      <c r="X41" s="8"/>
       <c r="Y41" s="6"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z41" s="6"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
+      <c r="C42" s="4"/>
       <c r="D42" s="7"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
@@ -6832,10 +7119,12 @@
       <c r="S42" s="4"/>
       <c r="T42" s="4"/>
       <c r="U42" s="7"/>
-      <c r="V42" s="46"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V42" s="7"/>
+      <c r="W42" s="35"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
+      <c r="C43" s="4"/>
       <c r="D43" s="7"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -6854,10 +7143,12 @@
       <c r="S43" s="4"/>
       <c r="T43" s="4"/>
       <c r="U43" s="7"/>
-      <c r="V43" s="46"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V43" s="7"/>
+      <c r="W43" s="35"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
+      <c r="C44" s="4"/>
       <c r="D44" s="7"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -6876,9 +7167,10 @@
       <c r="S44" s="4"/>
       <c r="T44" s="4"/>
       <c r="U44" s="7"/>
-      <c r="V44" s="46"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V44" s="7"/>
+      <c r="W44" s="35"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="4"/>
@@ -6898,9 +7190,10 @@
       <c r="S45" s="4"/>
       <c r="T45" s="4"/>
       <c r="U45" s="7"/>
-      <c r="V45" s="46"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V45" s="7"/>
+      <c r="W45" s="35"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="4"/>
@@ -6920,9 +7213,10 @@
       <c r="S46" s="4"/>
       <c r="T46" s="4"/>
       <c r="U46" s="7"/>
-      <c r="V46" s="46"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V46" s="7"/>
+      <c r="W46" s="35"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="4"/>
@@ -6942,9 +7236,10 @@
       <c r="S47" s="4"/>
       <c r="T47" s="4"/>
       <c r="U47" s="7"/>
-      <c r="V47" s="46"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V47" s="7"/>
+      <c r="W47" s="35"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="4"/>
@@ -6964,9 +7259,10 @@
       <c r="S48" s="4"/>
       <c r="T48" s="4"/>
       <c r="U48" s="7"/>
-      <c r="V48" s="46"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V48" s="7"/>
+      <c r="W48" s="35"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="4"/>
@@ -6986,9 +7282,10 @@
       <c r="S49" s="4"/>
       <c r="T49" s="4"/>
       <c r="U49" s="7"/>
-      <c r="V49" s="46"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V49" s="7"/>
+      <c r="W49" s="35"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="D50" s="7"/>
       <c r="E50" s="4"/>
@@ -7008,9 +7305,10 @@
       <c r="S50" s="4"/>
       <c r="T50" s="4"/>
       <c r="U50" s="7"/>
-      <c r="V50" s="46"/>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="V50" s="7"/>
+      <c r="W50" s="35"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="4"/>
@@ -7030,9 +7328,10 @@
       <c r="S51" s="4"/>
       <c r="T51" s="4"/>
       <c r="U51" s="7"/>
-      <c r="V51" s="46"/>
-    </row>
-    <row r="52" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V51" s="7"/>
+      <c r="W51" s="35"/>
+    </row>
+    <row r="52" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="4"/>
@@ -7052,22 +7351,310 @@
       <c r="S52" s="4"/>
       <c r="T52" s="4"/>
       <c r="U52" s="7"/>
-      <c r="V52" s="46"/>
-      <c r="W52" s="8"/>
-      <c r="X52" s="6"/>
+      <c r="V52" s="7"/>
+      <c r="W52" s="35"/>
+      <c r="X52" s="8"/>
       <c r="Y52" s="6"/>
+      <c r="Z52" s="6"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="4"/>
+      <c r="T53" s="4"/>
+      <c r="U53" s="7"/>
+      <c r="V53" s="7"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4"/>
+      <c r="U54" s="7"/>
+      <c r="V54" s="7"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+      <c r="U55" s="7"/>
+      <c r="V55" s="7"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="7"/>
+      <c r="V56" s="7"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="7"/>
+      <c r="V57" s="7"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4"/>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+      <c r="T58" s="4"/>
+      <c r="U58" s="7"/>
+      <c r="V58" s="7"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+      <c r="T59" s="4"/>
+      <c r="U59" s="7"/>
+      <c r="V59" s="7"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+      <c r="T60" s="4"/>
+      <c r="U60" s="7"/>
+      <c r="V60" s="7"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4"/>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+      <c r="T61" s="4"/>
+      <c r="U61" s="7"/>
+      <c r="V61" s="7"/>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4"/>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
+      <c r="T62" s="4"/>
+      <c r="U62" s="7"/>
+      <c r="V62" s="7"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4"/>
+      <c r="L63" s="4"/>
+      <c r="M63" s="4"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="4"/>
+      <c r="P63" s="4"/>
+      <c r="Q63" s="4"/>
+      <c r="R63" s="4"/>
+      <c r="S63" s="4"/>
+      <c r="T63" s="4"/>
+      <c r="U63" s="7"/>
+      <c r="V63" s="7"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="L64" s="4"/>
+      <c r="M64" s="4"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="4"/>
+      <c r="P64" s="4"/>
+      <c r="Q64" s="4"/>
+      <c r="R64" s="4"/>
+      <c r="S64" s="4"/>
+      <c r="T64" s="4"/>
+      <c r="U64" s="7"/>
+      <c r="V64" s="7"/>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="4"/>
+      <c r="L65" s="4"/>
+      <c r="M65" s="4"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="4"/>
+      <c r="P65" s="4"/>
+      <c r="Q65" s="4"/>
+      <c r="R65" s="4"/>
+      <c r="S65" s="4"/>
+      <c r="T65" s="4"/>
+      <c r="U65" s="7"/>
+      <c r="V65" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="Y1:Y2"/>
+  <mergeCells count="10">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Z1:Z2"/>
     <mergeCell ref="O1:U1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:N1"/>
-    <mergeCell ref="V1:V2"/>
     <mergeCell ref="W1:W2"/>
     <mergeCell ref="X1:X2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="Y1:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7076,318 +7663,682 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
+      <pane xSplit="8" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="140.85546875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="255.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="106.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="4" style="2" customWidth="1"/>
+    <col min="5" max="5" width="4" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="64.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="130.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="255.42578125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="85.5703125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="45"/>
+      <c r="H1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="I1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="J1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-    </row>
-    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
+    <row r="2" spans="1:11" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39"/>
+      <c r="B2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="31">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="6"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="6"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="6"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="6"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="6"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="6"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="15"/>
+    </row>
+    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+    </row>
+    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+    </row>
+    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+    </row>
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+    </row>
+    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+    </row>
+    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
+  <mergeCells count="7">
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizar estatus, casos y otros
</commit_message>
<xml_diff>
--- a/Casos Cartera/Administración.xlsx
+++ b/Casos Cartera/Administración.xlsx
@@ -9,31 +9,29 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" tabRatio="787" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" tabRatio="787" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Alta crédito manual" sheetId="15" r:id="rId1"/>
     <sheet name="Cuenta Corriente" sheetId="38" r:id="rId2"/>
     <sheet name="Lista Blanca" sheetId="16" r:id="rId3"/>
-    <sheet name="Parámetros" sheetId="17" r:id="rId4"/>
-    <sheet name="Parámetros de asignación" sheetId="20" r:id="rId5"/>
-    <sheet name="Tasa Máxima Convencional" sheetId="21" r:id="rId6"/>
-    <sheet name="Parámetros Afianza" sheetId="22" r:id="rId7"/>
-    <sheet name="Criterio Selección Crédito (Afi" sheetId="23" r:id="rId8"/>
-    <sheet name="Exclusión Tipo Vehículo (Afianz" sheetId="24" r:id="rId9"/>
-    <sheet name="Documentos Requeridos (Afianza)" sheetId="25" r:id="rId10"/>
-    <sheet name="Parámetros CRM SAC" sheetId="26" r:id="rId11"/>
+    <sheet name="Parámetros de asignación" sheetId="20" r:id="rId4"/>
+    <sheet name="Tasa Máxima Convencional" sheetId="21" r:id="rId5"/>
+    <sheet name="Parámetros Afianza" sheetId="22" r:id="rId6"/>
+    <sheet name="Criterio Selección Crédito (Afi" sheetId="23" r:id="rId7"/>
+    <sheet name="Exclusión Tipo Vehículo (Afianz" sheetId="24" r:id="rId8"/>
+    <sheet name="Documentos Requeridos (Afianza)" sheetId="25" r:id="rId9"/>
+    <sheet name="Parámetros CRM SAC" sheetId="26" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Alta crédito manual'!$A$2:$H$50</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="219">
   <si>
     <t>Nombre CP</t>
   </si>
@@ -56,63 +54,6 @@
     <t>Modificar</t>
   </si>
   <si>
-    <t>TC_Cartera_ProcesoXML_OfertaTD</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesoXML_RestoXML</t>
-  </si>
-  <si>
-    <t>TC_Cartera_ProcesoXML_CartaGuiaID</t>
-  </si>
-  <si>
-    <t>Validar emisión XML con la opción oferta y TD</t>
-  </si>
-  <si>
-    <t>Validar emisión XML con la opción resto XML</t>
-  </si>
-  <si>
-    <t>Validar emisión XML, sin indicar ID de carta guía</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Generación XML (afianza), ingresar ID válido de carta guía, hacer clic en boton Generar XML Oferta y TD</t>
-  </si>
-  <si>
-    <t>XML generado exitosamente</t>
-  </si>
-  <si>
-    <t>Sisteme emite mensaje indicando "Debe ingresar Carta Guia"</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Generación XML (afianza), ingresar ID válido de carta guía, hacer clic en boton Resto XML</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Generación XML (afianza), hacer clic en boton Generar XML Oferta y TD</t>
-  </si>
-  <si>
-    <t>TC_Cartera_CentralizacionCreditosNuevos_FechaError</t>
-  </si>
-  <si>
-    <t>TC_Cartera_CentralizacionCreditosNuevos_Generar</t>
-  </si>
-  <si>
-    <t>Validar emisión de archivo excel contabilización, el cual es cargado en sistema Softland para generar los comprobantes contables por cada crédito enviado a él.</t>
-  </si>
-  <si>
-    <t>Validar emisión de archivo excel contabilización, sin indicar fecha para genera contabilización.</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Centralización Créditos Nuevos, ingresar fecha, hacer clic en botón generar contabilización</t>
-  </si>
-  <si>
-    <t>Emisión de archivo excel con formato exigido por Softland</t>
-  </si>
-  <si>
-    <t>Sistema emite mensaje indicando Debe ingresar una fecha.</t>
-  </si>
-  <si>
-    <t>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Proceso - sub modulo Centralización Créditos Nuevos, hacer clic en botón generar contabilización</t>
-  </si>
-  <si>
     <t>Validar decarga de archivo con formato solicitado por la SBIF, sin indicar mes y año</t>
   </si>
   <si>
@@ -735,6 +676,18 @@
   </si>
   <si>
     <t>Validar respueda de web service, inidicando login y contraseña correctos</t>
+  </si>
+  <si>
+    <t>TC_Cartera_AdministracionPAfianza_FTP</t>
+  </si>
+  <si>
+    <t>Validar envío de archvio a directorio configurado</t>
+  </si>
+  <si>
+    <t>Acceder a directorio configurado para visualizar archivo enviado</t>
+  </si>
+  <si>
+    <t>Archivo enviado a directorio configurado</t>
   </si>
 </sst>
 </file>
@@ -1318,86 +1271,86 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1594,330 +1547,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="52.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="176.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="255.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="85.5703125" style="6" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
-        <v>215</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>221</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>222</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="35"/>
-      <c r="D13" s="15"/>
-    </row>
-    <row r="14" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="15"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="35"/>
-      <c r="D15" s="15"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="D16" s="15"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="35"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="D18" s="15"/>
-    </row>
-    <row r="19" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="15"/>
-    </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="15"/>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="35"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="35"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="35"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="35"/>
-      <c r="C32" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
-    </row>
-    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="35"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="35"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="35"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="35"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="35"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="35"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="35"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="35"/>
-    </row>
-    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A1:A2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1951,44 +1583,44 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>233</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2234,19 +1866,19 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C1" s="42"/>
       <c r="D1" s="42"/>
       <c r="E1" s="43" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F1" s="44"/>
       <c r="G1" s="45" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="H1" s="46"/>
       <c r="I1" s="37" t="s">
@@ -2274,10 +1906,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>6</v>
@@ -2308,7 +1940,7 @@
       </c>
       <c r="H3" s="7"/>
       <c r="I3" s="6" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="J3" s="8" t="str">
         <f>CONCATENATE("Validar funcionalidad ",IF(B3=1,$B$2,IF(C3=1,$C$2,IF(D3=1,$D$2))),", considerando el enlace ",IF(E3=1,$E$2,IF(F3=1,$F$2,""))," para realizar la acción de ",IF(G3=1,$G$2,IF(H3=1,$H$2,"")))</f>
@@ -2319,7 +1951,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton agregar, considerar enlace Corriente Nro para realizar la acción de modificar registro</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2340,7 +1972,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="J4" s="8" t="str">
         <f t="shared" ref="J4:J16" si="0">CONCATENATE("Validar funcionalidad ",IF(B4=1,$B$2,IF(C4=1,$C$2,IF(D4=1,$D$2))),", considerando el enlace ",IF(E4=1,$E$2,IF(F4=1,$F$2,""))," para realizar la acción de ",IF(G4=1,$G$2,IF(H4=1,$H$2,"")))</f>
@@ -2351,7 +1983,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton agregar, considerar enlace Corriente Nro para realizar la acción de eliminar registro</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2372,7 +2004,7 @@
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="6" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="J5" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2383,7 +2015,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton agregar, considerar enlace Banco para realizar la acción de modificar registro</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2404,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="J6" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2415,7 +2047,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton agregar, considerar enlace Banco para realizar la acción de eliminar registro</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2432,17 +2064,17 @@
       <c r="G7" s="4"/>
       <c r="H7" s="7"/>
       <c r="I7" s="6" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="K7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton agregar</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -2463,7 +2095,7 @@
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="6" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="J8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2474,7 +2106,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton eliminar, considerar enlace Corriente Nro para realizar la acción de modificar registro</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2494,7 +2126,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="J9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2505,7 +2137,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton eliminar, considerar enlace Corriente Nro para realizar la acción de eliminar registro</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2525,7 +2157,7 @@
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="6" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="J10" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2536,7 +2168,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton eliminar, considerar enlace Banco para realizar la acción de modificar registro</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2556,7 +2188,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="J11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2567,7 +2199,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton eliminar, considerar enlace Banco para realizar la acción de eliminar registro</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2583,17 +2215,17 @@
       <c r="G12" s="4"/>
       <c r="H12" s="7"/>
       <c r="I12" s="6" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="K12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton eliminar</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2612,7 +2244,7 @@
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="6" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="J13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2623,7 +2255,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton modificar, considerar enlace Corriente Nro para realizar la acción de modificar registro</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2642,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="J14" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2653,7 +2285,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton modificar, considerar enlace Corriente Nro para realizar la acción de eliminar registro</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2672,7 +2304,7 @@
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="6" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="J15" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2683,7 +2315,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton modificar, considerar enlace Banco para realizar la acción de modificar registro</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2702,7 +2334,7 @@
         <v>1</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="J16" s="8" t="str">
         <f t="shared" si="0"/>
@@ -2713,7 +2345,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton modificar, considerar enlace Banco para realizar la acción de eliminar registro</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2728,17 +2360,17 @@
       <c r="G17" s="4"/>
       <c r="H17" s="7"/>
       <c r="I17" s="6" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="J17" s="8" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="K17" s="6" t="str">
         <f t="shared" si="1"/>
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Cuenta Corriente, hacer clic en boton modificar</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2920,16 +2552,16 @@
       <c r="G32" s="4"/>
       <c r="H32" s="7"/>
       <c r="I32" s="6" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
@@ -3174,22 +2806,22 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C1" s="42"/>
       <c r="D1" s="42"/>
       <c r="E1" s="25" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="G1" s="46"/>
       <c r="H1" s="39" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="I1" s="37" t="s">
         <v>0</v>
@@ -3216,7 +2848,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -3248,16 +2880,16 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="6" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3278,16 +2910,16 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="6" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3306,16 +2938,16 @@
         <v>1</v>
       </c>
       <c r="I5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3332,16 +2964,16 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="6" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -3360,16 +2992,16 @@
         <v>1</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3385,16 +3017,16 @@
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="6" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>114</v>
+        <v>95</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3412,16 +3044,16 @@
         <v>1</v>
       </c>
       <c r="I9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L9" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3465,16 +3097,16 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="6" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3896,294 +3528,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="52.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="168.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="192.140625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="79" style="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-    </row>
-    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="9" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD1048576"/>
+      <selection pane="topRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4204,22 +3553,22 @@
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C1" s="42"/>
       <c r="D1" s="44"/>
       <c r="E1" s="30" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="G1" s="46"/>
       <c r="H1" s="39" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="I1" s="37" t="s">
         <v>0</v>
@@ -4246,7 +3595,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -4278,16 +3627,16 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>122</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4308,16 +3657,16 @@
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="6" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>135</v>
+        <v>116</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4336,16 +3685,16 @@
         <v>1</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>130</v>
+        <v>111</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4364,16 +3713,16 @@
         <v>1</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4392,16 +3741,16 @@
         <v>1</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -4427,16 +3776,16 @@
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="6" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4922,7 +4271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
@@ -4961,16 +4310,16 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -4996,6 +4345,285 @@
       <c r="B7" s="8"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="C16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+    </row>
+    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+    </row>
+    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+    </row>
+    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+    </row>
+    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.7109375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="95.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="9" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="15"/>
     </row>
     <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
@@ -5202,301 +4830,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D50"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="51.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="255.42578125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="79" style="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="C10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="C14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="C15" s="8"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="15"/>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-    </row>
-    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-    </row>
-    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-    </row>
-    <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-    </row>
-    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A1:A2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z65"/>
   <sheetViews>
@@ -5533,20 +4866,20 @@
   <sheetData>
     <row r="1" spans="1:26" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C1" s="42"/>
       <c r="D1" s="42"/>
       <c r="E1" s="43" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="F1" s="49"/>
       <c r="G1" s="44"/>
       <c r="H1" s="45" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="I1" s="48"/>
       <c r="J1" s="48"/>
@@ -5555,7 +4888,7 @@
       <c r="M1" s="48"/>
       <c r="N1" s="46"/>
       <c r="O1" s="45" t="s">
-        <v>149</v>
+        <v>130</v>
       </c>
       <c r="P1" s="48"/>
       <c r="Q1" s="48"/>
@@ -5564,7 +4897,7 @@
       <c r="T1" s="48"/>
       <c r="U1" s="46"/>
       <c r="V1" s="47" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="W1" s="50" t="s">
         <v>0</v>
@@ -5591,55 +4924,55 @@
         <v>6</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>179</v>
+        <v>160</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>146</v>
+        <v>127</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>147</v>
+        <v>128</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="Q2" s="11" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="R2" s="11" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="U2" s="29" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="V2" s="38"/>
       <c r="W2" s="40"/>
@@ -5683,7 +5016,7 @@
         <v>1</v>
       </c>
       <c r="W3" s="35" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="X3" s="8" t="str">
         <f>CONCATENATE("Validad funcionalidad ",IF(B3=1,$B$2,IF(C3=1,$C$2,IF(D3=1,$D$2))),IF(B3=1,", ingresando registro ",IF(C3=1,", seleccionando registro ",IF(D3=1,", seleccionando registro "))),$E$1," ",IF(E3=1,$E$2,IF(F3=1,$F$2,IF(G3=1,$G$2))),"y ",$H$1," ",IF(H3=1,$H$2,IF(I3=1,$I$2,IF(J3=1,$J$2,IF(K3=1,$K$2,IF(L3=1,$L$2,IF(M3=1,$M$2,IF(N3=1,$N$2)))))))," - ",$O$1," ",IF(O3=1,$O$2,IF(P3=1,$P$2,IF(Q3=1,$Q$2,IF(R3=1,$R$2,IF(S3=1,$S$2,IF(T3=1,$T$2,IF(U3=1,$U$2))))))),IF(V3=1,". Considerando la opcion de exportar a excel",""))</f>
@@ -5694,7 +5027,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Numerico y Operador Desde Igual - Operador Hasta No Aplica, finalizando con exportar a excel</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5731,7 +5064,7 @@
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="35" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="X4" s="8" t="str">
         <f t="shared" ref="X4:X5" si="0">CONCATENATE("Validad funcionalidad ",IF(B4=1,$B$2,IF(C4=1,$C$2,IF(D4=1,$D$2))),IF(B4=1,", ingresando registro ",IF(C4=1,", seleccionando registro ",IF(D4=1,", seleccionando registro "))),$E$1," ",IF(E4=1,$E$2,IF(F4=1,$F$2,IF(G4=1,$G$2))),"y ",$H$1," ",IF(H4=1,$H$2,IF(I4=1,$I$2,IF(J4=1,$J$2,IF(K4=1,$K$2,IF(L4=1,$L$2,IF(M4=1,$M$2,IF(N4=1,$N$2)))))))," - ",$O$1," ",IF(O4=1,$O$2,IF(P4=1,$P$2,IF(Q4=1,$Q$2,IF(R4=1,$R$2,IF(S4=1,$S$2,IF(T4=1,$T$2,IF(U4=1,$U$2))))))),IF(V4=1,". Considerando la opcion de exportar a excel",""))</f>
@@ -5742,7 +5075,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Numerico y Operador Desde Mayor - Operador Hasta Distinto</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5779,7 +5112,7 @@
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
       <c r="W5" s="35" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="X5" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5790,7 +5123,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Numerico y Operador Desde Menor - Operador Hasta Menor igual</v>
       </c>
       <c r="Z5" s="6" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5829,7 +5162,7 @@
         <v>1</v>
       </c>
       <c r="W6" s="35" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="X6" s="8" t="str">
         <f>CONCATENATE("Validad funcionalidad ",IF(B6=1,$B$2,IF(C6=1,$C$2,IF(D6=1,$D$2))),IF(B6=1,", ingresando registro ",IF(C6=1,", seleccionando registro ",IF(D6=1,", seleccionando registro "))),$E$1," ",IF(E6=1,$E$2,IF(F6=1,$F$2,IF(G6=1,$G$2)))," y ",$H$1," ",IF(H6=1,$H$2,IF(I6=1,$I$2,IF(J6=1,$J$2,IF(K6=1,$K$2,IF(L6=1,$L$2,IF(M6=1,$M$2,IF(N6=1,$N$2)))))))," - ",$O$1," ",IF(O6=1,$O$2,IF(P6=1,$P$2,IF(Q6=1,$Q$2,IF(R6=1,$R$2,IF(S6=1,$S$2,IF(T6=1,$T$2,IF(U6=1,$U$2))))))),IF(V6=1,". Considerando la opcion de exportar a excel",""))</f>
@@ -5840,7 +5173,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Fecha y Operador Desde Mayor igual - Operador Hasta Mayor igual, finalizando con exportar a excel</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5877,7 +5210,7 @@
       <c r="U7" s="7"/>
       <c r="V7" s="7"/>
       <c r="W7" s="35" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="X7" s="8" t="str">
         <f t="shared" ref="X7:X22" si="2">CONCATENATE("Validad funcionalidad ",IF(B7=1,$B$2,IF(C7=1,$C$2,IF(D7=1,$D$2))),IF(B7=1,", ingresando registro ",IF(C7=1,", seleccionando registro ",IF(D7=1,", seleccionando registro "))),$E$1," ",IF(E7=1,$E$2,IF(F7=1,$F$2,IF(G7=1,$G$2)))," y ",$H$1," ",IF(H7=1,$H$2,IF(I7=1,$I$2,IF(J7=1,$J$2,IF(K7=1,$K$2,IF(L7=1,$L$2,IF(M7=1,$M$2,IF(N7=1,$N$2)))))))," - ",$O$1," ",IF(O7=1,$O$2,IF(P7=1,$P$2,IF(Q7=1,$Q$2,IF(R7=1,$R$2,IF(S7=1,$S$2,IF(T7=1,$T$2,IF(U7=1,$U$2))))))),IF(V7=1,". Considerando la opcion de exportar a excel",""))</f>
@@ -5888,7 +5221,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Fecha y Operador Desde Menor igual - Operador Hasta Menor</v>
       </c>
       <c r="Z7" s="6" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -5925,7 +5258,7 @@
       <c r="U8" s="7"/>
       <c r="V8" s="7"/>
       <c r="W8" s="35" t="s">
-        <v>163</v>
+        <v>144</v>
       </c>
       <c r="X8" s="8" t="str">
         <f t="shared" si="2"/>
@@ -5936,7 +5269,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Carácter y Operador Desde Distinto - Operador Hasta Mayor</v>
       </c>
       <c r="Z8" s="6" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5975,7 +5308,7 @@
         <v>1</v>
       </c>
       <c r="W9" s="35" t="s">
-        <v>164</v>
+        <v>145</v>
       </c>
       <c r="X9" s="8" t="str">
         <f t="shared" si="2"/>
@@ -5986,7 +5319,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), hacer clic en boton agregar e ingresar Tipo dato Carácter y Operador Desde No Aplica - Operador Hasta Igual, finalizando con exportar a excel</v>
       </c>
       <c r="Z9" s="6" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6023,7 +5356,7 @@
       </c>
       <c r="V10" s="7"/>
       <c r="W10" s="35" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="X10" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6034,7 +5367,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Fecha y Operador Desde Igual - Operador Hasta No Aplica para eliminar</v>
       </c>
       <c r="Z10" s="15" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
@@ -6071,7 +5404,7 @@
       <c r="U11" s="7"/>
       <c r="V11" s="7"/>
       <c r="W11" s="35" t="s">
-        <v>166</v>
+        <v>147</v>
       </c>
       <c r="X11" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6082,7 +5415,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Fecha y Operador Desde Mayor - Operador Hasta Distinto para eliminar</v>
       </c>
       <c r="Z11" s="15" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -6121,7 +5454,7 @@
         <v>1</v>
       </c>
       <c r="W12" s="35" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="X12" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6132,7 +5465,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Fecha y Operador Desde Menor - Operador Hasta Menor igual para eliminar, finalizando con exportar a excel</v>
       </c>
       <c r="Z12" s="15" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -6169,7 +5502,7 @@
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
       <c r="W13" s="35" t="s">
-        <v>168</v>
+        <v>149</v>
       </c>
       <c r="X13" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6180,7 +5513,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Carácter y Operador Desde Mayor igual - Operador Hasta Mayor igual para eliminar</v>
       </c>
       <c r="Z13" s="15" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -6217,7 +5550,7 @@
       <c r="U14" s="7"/>
       <c r="V14" s="7"/>
       <c r="W14" s="35" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="X14" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6228,7 +5561,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Carácter y Operador Desde Menor igual - Operador Hasta Menor para eliminar</v>
       </c>
       <c r="Z14" s="15" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
@@ -6267,7 +5600,7 @@
         <v>1</v>
       </c>
       <c r="W15" s="35" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="X15" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6278,7 +5611,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Numerico y Operador Desde Distinto - Operador Hasta Mayor para eliminar, finalizando con exportar a excel</v>
       </c>
       <c r="Z15" s="15" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -6315,7 +5648,7 @@
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
       <c r="W16" s="35" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="X16" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6326,7 +5659,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registro Tipo dato Numerico y Operador Desde No Aplica - Operador Hasta Igual para eliminar</v>
       </c>
       <c r="Z16" s="15" t="s">
-        <v>181</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
@@ -6362,7 +5695,7 @@
       </c>
       <c r="V17" s="7"/>
       <c r="W17" s="35" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="X17" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6373,7 +5706,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Carácter y Operador Desde Igual - Operador Hasta No Aplica para modificar</v>
       </c>
       <c r="Z17" s="15" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -6411,7 +5744,7 @@
         <v>1</v>
       </c>
       <c r="W18" s="35" t="s">
-        <v>173</v>
+        <v>154</v>
       </c>
       <c r="X18" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6422,7 +5755,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Carácter y Operador Desde Mayor - Operador Hasta Distinto para modificar, finalizando con exportar a excel</v>
       </c>
       <c r="Z18" s="15" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -6458,7 +5791,7 @@
       <c r="U19" s="7"/>
       <c r="V19" s="7"/>
       <c r="W19" s="35" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="X19" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6469,7 +5802,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Carácter y Operador Desde Menor - Operador Hasta Menor igual para modificar</v>
       </c>
       <c r="Z19" s="15" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6505,7 +5838,7 @@
       <c r="U20" s="7"/>
       <c r="V20" s="7"/>
       <c r="W20" s="35" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="X20" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6516,7 +5849,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Fecha y Operador Desde Mayor igual - Operador Hasta Mayor igual para modificar</v>
       </c>
       <c r="Z20" s="15" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6555,7 +5888,7 @@
         <v>1</v>
       </c>
       <c r="W21" s="35" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="X21" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6566,7 +5899,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Fecha y Operador Desde Menor igual - Operador Hasta Menor para modificar, finalizando con exportar a excel</v>
       </c>
       <c r="Z21" s="15" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6603,7 +5936,7 @@
       <c r="U22" s="7"/>
       <c r="V22" s="7"/>
       <c r="W22" s="35" t="s">
-        <v>177</v>
+        <v>158</v>
       </c>
       <c r="X22" s="8" t="str">
         <f t="shared" si="2"/>
@@ -6614,7 +5947,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Numerico y Operador Desde Distinto - Operador Hasta Mayor para modificar</v>
       </c>
       <c r="Z22" s="15" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6651,7 +5984,7 @@
       <c r="U23" s="7"/>
       <c r="V23" s="7"/>
       <c r="W23" s="35" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
       <c r="X23" s="8" t="str">
         <f>CONCATENATE("Validad funcionalidad ",IF(B23=1,$B$2,IF(C23=1,$C$2,IF(D23=1,$D$2))),IF(B23=1,", ingresando registro ",IF(C23=1,", seleccionando registro ",IF(D23=1,", seleccionando registro "))),$E$1," ",IF(E23=1,$E$2,IF(F23=1,$F$2,IF(G23=1,$G$2)))," y ",$H$1," ",IF(H23=1,$H$2,IF(I23=1,$I$2,IF(J23=1,$J$2,IF(K23=1,$K$2,IF(L23=1,$L$2,IF(M23=1,$M$2,IF(N23=1,$N$2)))))))," - ",$O$1," ",IF(O23=1,$O$2,IF(P23=1,$P$2,IF(Q23=1,$Q$2,IF(R23=1,$R$2,IF(S23=1,$S$2,IF(T23=1,$T$2,IF(U23=1,$U$2))))))),IF(V23=1,". Considerando la opcion de exportar a excel",""))</f>
@@ -6662,7 +5995,7 @@
         <v>Acceder a sistema Cartera con usuario que posee perfil para acceder al modulo Administración - sub modulo Criterio Selección Crédito (Afianza), seleccionar registroTipo dato Numerico y Operador Desde No Aplica - Operador Hasta Igual para modificar</v>
       </c>
       <c r="Z23" s="15" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6900,16 +6233,16 @@
       <c r="U32" s="7"/>
       <c r="V32" s="7"/>
       <c r="W32" s="35" t="s">
-        <v>183</v>
+        <v>164</v>
       </c>
       <c r="X32" s="8" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="Y32" s="6" t="s">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="Z32" s="6" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
@@ -7709,7 +7042,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
@@ -7735,18 +7068,18 @@
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="39" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C1" s="42"/>
       <c r="D1" s="44"/>
       <c r="E1" s="30" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="G1" s="46"/>
       <c r="H1" s="37" t="s">
@@ -7774,7 +7107,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>6</v>
@@ -7804,16 +7137,16 @@
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="6" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7833,16 +7166,16 @@
         <v>1</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7858,16 +7191,16 @@
       <c r="F5" s="4"/>
       <c r="G5" s="7"/>
       <c r="H5" s="6" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7883,16 +7216,16 @@
       <c r="F6" s="4"/>
       <c r="G6" s="7"/>
       <c r="H6" s="6" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -7908,16 +7241,16 @@
       <c r="F7" s="4"/>
       <c r="G7" s="7"/>
       <c r="H7" s="6" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -7941,16 +7274,16 @@
       <c r="F9" s="4"/>
       <c r="G9" s="7"/>
       <c r="H9" s="6" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -8390,4 +7723,325 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D52"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="176.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="255.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="85.5703125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="9" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="40"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="35"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="35"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="35"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="35"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="35"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="35"/>
+      <c r="D13" s="15"/>
+    </row>
+    <row r="14" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="35"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="15"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="35"/>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="35"/>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="35"/>
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="35"/>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="15"/>
+    </row>
+    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="15"/>
+    </row>
+    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="35"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="35"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="35"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="35"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="35"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="35"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="35"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="35"/>
+      <c r="C32" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="35"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="35"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="35"/>
+    </row>
+    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="35"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+    </row>
+    <row r="37" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+    </row>
+    <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="35"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="35"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+    </row>
+    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="35"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="35"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="35"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="35"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="35"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="35"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="35"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="35"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="35"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="35"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="35"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="35"/>
+    </row>
+    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="35"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>